<commit_message>
general adjustments of the code
</commit_message>
<xml_diff>
--- a/scripts/BFI assessment module TRIAL2copy.xlsx
+++ b/scripts/BFI assessment module TRIAL2copy.xlsx
@@ -769,7 +769,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="20"/>
@@ -1126,10 +1126,10 @@
   <dimension ref="A1:BO47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="13.29"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="AC4" s="38" t="str">
         <f aca="false">Raw_Data!AB1</f>
-        <v>Io mi vedo come una persona che....17. Per natura tende a perdonare </v>
+        <v>Io mi vedo come una persona che....17. Per natura tende a perdonare</v>
       </c>
       <c r="AD4" s="39" t="str">
         <f aca="false">Raw_Data!AC1</f>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="BC4" s="39" t="str">
         <f aca="false">Raw_Data!BB1</f>
-        <v>Io mi vedo come una persona che....43. È facilmente distratta </v>
+        <v>Io mi vedo come una persona che....43. È facilmente distratta</v>
       </c>
       <c r="BD4" s="42" t="str">
         <f aca="false">Raw_Data!BC1</f>
@@ -4454,7 +4454,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>